<commit_message>
c section data and modified addStudents and addCourses
</commit_message>
<xml_diff>
--- a/server/tempCourse.xlsx
+++ b/server/tempCourse.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CO-PO\co_po_web\server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Express_projects\co_po_web\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD06AC07-B659-425D-96ED-F6BE7CCBF9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F15252-9866-45D9-939D-46E6EF08256E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="1908" windowWidth="18144" windowHeight="11052" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>coStatements</t>
   </si>
   <si>
-    <t>good theory-2, better lab-3</t>
-  </si>
-  <si>
     <t>Computer Networks</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>B.Tech</t>
   </si>
   <si>
-    <t>learn packet tracer-2, implement TCP-1</t>
-  </si>
-  <si>
     <t>CS501</t>
   </si>
   <si>
@@ -91,6 +85,12 @@
   </si>
   <si>
     <t>Lab</t>
+  </si>
+  <si>
+    <t>good theory#2| better lab#3</t>
+  </si>
+  <si>
+    <t>learn packet tracer#2| implement TCP#1</t>
   </si>
 </sst>
 </file>
@@ -417,12 +417,12 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,18 +451,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -477,21 +477,21 @@
         <v>9</v>
       </c>
       <c r="I2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -506,21 +506,21 @@
         <v>9</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -535,7 +535,7 @@
         <v>9</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>